<commit_message>
Update Exported Points of Intersections (MATLAB LiDAR Simulation).xlsx
</commit_message>
<xml_diff>
--- a/Exported Points of Intersections (MATLAB LiDAR Simulation).xlsx
+++ b/Exported Points of Intersections (MATLAB LiDAR Simulation).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Point of Intersection (x)</t>
   </si>
@@ -105,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -116,15 +116,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,351 +141,351 @@
   <dimension ref="A1:H13"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="true"/>
-    <col min="2" max="2" width="22.140625" customWidth="true"/>
-    <col min="3" max="3" width="22" customWidth="true"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true"/>
-    <col min="5" max="5" width="13.5703125" customWidth="true"/>
-    <col min="6" max="6" width="16.7109375" customWidth="true"/>
-    <col min="7" max="7" width="16.7109375" customWidth="true"/>
-    <col min="8" max="8" width="16.5703125" customWidth="true"/>
+    <col min="1" max="1" width="19.7109375" customWidth="true"/>
+    <col min="2" max="2" width="19.7109375" customWidth="true"/>
+    <col min="3" max="3" width="19.578125" customWidth="true"/>
+    <col min="4" max="4" width="11.64453125" customWidth="true"/>
+    <col min="5" max="5" width="12.11328125" customWidth="true"/>
+    <col min="6" max="6" width="14.77734375" customWidth="true"/>
+    <col min="7" max="7" width="14.77734375" customWidth="true"/>
+    <col min="8" max="8" width="14.64453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>0.8017608355259469</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>-0.030178641419321695</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>0.2053329502257637</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>293.58858239999012</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>-5</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>0.78778261047055786</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>-0.014195444789424836</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>0.20325235540914291</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>1.7804181670523069</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>-0.031771324660552658</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>0.45008350070370962</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>658.26017280030271</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>-3</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>1.7665691518065689</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>-0.033068193280980679</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>0.43390619766813948</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>2.7587751171080113</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>-0.070344289138308397</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>0.63177613232411323</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>1024.5242880005826</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>-1</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>2.7499591722707195</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>-0.053403323178024882</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>0.64128744211605782</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>2.7662521430909699</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>-0.042224620905375931</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>0.63160309102098644</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>1024.9224192005811</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>-1</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>2.7510282903330712</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>-0.05342617850138294</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>0.64149963787477138</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>4.7631486154724865</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>-0.10889621359590092</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>1.005079986699398</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>1770.5558015977499</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>7</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>4.7538777903325009</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>-0.09908429937196632</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>0.98855847449603229</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>5.7681504391161873</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>-0.1341810283211004</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>1.1170319009566503</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>2153.8897919973224</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>11</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>5.7839428107947963</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>-0.12477292234627589</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>1.127861063608081</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>5.7841301673448013</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>-0.14186610873143252</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <v>1.1152183726450835</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>2154.2879231973247</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>11</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>5.7850127566092278</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>-0.12480038333906153</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>1.127991949983578</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>5.7987995115535549</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>-0.13684910071526771</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9">
         <v>1.11591811888008</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9">
         <v>2154.6860543973271</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>11</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>5.7860827026573025</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>-0.12482784595120645</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>1.12812280774927</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>6.8165867434853658</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>-0.15671522730238455</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10">
         <v>1.2220832927695964</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>2540.8567295996099</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10">
         <v>13</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>6.823989642797117</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>-0.15222770408142375</v>
       </c>
-      <c r="H10" s="0">
+      <c r="H10">
         <v>1.2415830733355775</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>6.8328362043698645</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>-0.15890300580916056</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11">
         <v>1.2229635414535738</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11">
         <v>2541.2548607996123</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11">
         <v>13</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>6.8250597966464168</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>-0.15225673819980498</v>
       </c>
-      <c r="H11" s="0">
+      <c r="H11">
         <v>1.2416861704031505</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>7.8325993671370613</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12">
         <v>-0.19348897236500553</v>
       </c>
-      <c r="C12" s="0">
+      <c r="C12">
         <v>1.3376736299940446</v>
       </c>
-      <c r="D12" s="0">
+      <c r="D12">
         <v>2921.0222592018572</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12">
         <v>13</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>7.845935566038694</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>-0.18068831483537842</v>
       </c>
-      <c r="H12" s="0">
+      <c r="H12">
         <v>1.3270213442925958</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>8.8306897235909734</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>-0.21986440678473693</v>
       </c>
-      <c r="C13" s="0">
+      <c r="C13">
         <v>1.3775656241837562</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D13">
         <v>3293.6896512040603</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13">
         <v>11</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>8.8478638919494124</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>-0.21001888967481236</v>
       </c>
-      <c r="H13" s="0">
+      <c r="H13">
         <v>1.3855214999390835</v>
       </c>
     </row>

</xml_diff>